<commit_message>
Select Enhanced and Flag Hunter
</commit_message>
<xml_diff>
--- a/Python/litigation/LITTY/LITTY - REF - cópia/PLANILHA REFERENCIA - COM CELULA COMPOSTA.xlsx
+++ b/Python/litigation/LITTY/LITTY - REF - cópia/PLANILHA REFERENCIA - COM CELULA COMPOSTA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joao/Projetos/repo/personal-academy/Python/litigation/LITTY/LITTY - REF - cópia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF0BA51-A55D-8348-A16E-5D242F9D3552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFC230E-0D57-AC4A-B998-FF9BCCB58903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12580" yWindow="1140" windowWidth="21200" windowHeight="11200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>NACIONALIDADE</t>
   </si>
@@ -127,12 +127,33 @@
   </si>
   <si>
     <t>NU Bank, C6 Bank, Banrisul, SWEAT, Itaú, Banco do Brasil, Santander, Picpay, Mercado Pago, Pagbank, Cirrus</t>
+  </si>
+  <si>
+    <t>VALOR DE CAUSA</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>CNPJS</t>
+  </si>
+  <si>
+    <t>ENDEREÇO BANCOS</t>
+  </si>
+  <si>
+    <t>R. Machado de Assis, Av. Bossa Nova, R. Canários, R. Catamarã, Av. Cristovão Colombo, Av. Oliveria Nunes, R. Parque das Águas</t>
+  </si>
+  <si>
+    <t>33.010.284/0001-56, 19.041.377/0001-17, 90.261.648/0001-04, 22.611.216/0001-26, 45.279.812/0001-56, 13.902.317/0001-65</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,10 +204,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -502,15 +525,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -648,6 +671,38 @@
       </c>
       <c r="B17" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="3">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="4">
+        <v>44776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>